<commit_message>
Added actual xls and xlsx examples
</commit_message>
<xml_diff>
--- a/t/data/test.xlsx
+++ b/t/data/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="21075" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="21075" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="simple" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>A</t>
   </si>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t>Meta Header</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xyz  </t>
   </si>
 </sst>
 </file>
@@ -583,7 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -608,41 +620,41 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
+      <c r="C4" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -654,7 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>